<commit_message>
Committing Task 17 and Notes on Chap15
</commit_message>
<xml_diff>
--- a/DTS350TemplateMaster/Week_08/Class_Task_15/15Task DB Schematic.xlsx
+++ b/DTS350TemplateMaster/Week_08/Class_Task_15/15Task DB Schematic.xlsx
@@ -8,14 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\000 DTS 350 Data Visualization\DTS350-hollinbergert\DTS350TemplateMaster\Week_08\Class_Task_15\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6194FB76-DE52-42B0-B752-3D9FCB1109D9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66882F66-98CF-453B-92D3-F049F6EB6688}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29550" yWindow="1590" windowWidth="16350" windowHeight="14010" xr2:uid="{6FCCE5E6-59F0-47E6-9422-CEE927A4B982}"/>
+    <workbookView xWindow="30975" yWindow="1890" windowWidth="16350" windowHeight="14010" xr2:uid="{6FCCE5E6-59F0-47E6-9422-CEE927A4B982}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$2:$P$37</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -1846,7 +1849,7 @@
   <dimension ref="A3:W144"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="A2" sqref="A2:P37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3355,7 +3358,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="64" orientation="landscape" r:id="rId1"/>
+  <pageSetup scale="71" orientation="landscape" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>

</xml_diff>